<commit_message>
these files will change every time a new .csv file is downloaded
</commit_message>
<xml_diff>
--- a/workouts.xlsx
+++ b/workouts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,47 +449,32 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>superset_id</t>
+          <t>set_index</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>exercise_notes</t>
+          <t>set_type</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>set_index</t>
+          <t>weight_lbs</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>set_type</t>
+          <t>reps</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>weight_lbs</t>
+          <t>distance_miles</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>reps</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>distance_miles</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
           <t>duration_seconds</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>rpe</t>
         </is>
       </c>
     </row>
@@ -519,31 +504,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -571,31 +553,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -623,31 +602,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -675,31 +651,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -727,31 +700,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -779,31 +749,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -827,31 +794,28 @@
           <t>Lat Pulldown (Cable)</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -875,31 +839,28 @@
           <t>Lat Pulldown (Cable)</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -923,31 +884,28 @@
           <t>Lat Pulldown (Cable)</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -971,31 +929,28 @@
           <t>Bicep Curl (Machine)</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1019,31 +974,28 @@
           <t>Bicep Curl (Machine)</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>30.0</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1067,31 +1019,28 @@
           <t>Bicep Curl (Machine)</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>25.0</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1115,31 +1064,28 @@
           <t>T Bar Row</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>25.0</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1163,31 +1109,28 @@
           <t>Hammer Curl (Cable)</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1211,31 +1154,28 @@
           <t>Hammer Curl (Cable)</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1259,31 +1199,28 @@
           <t>Hammer Curl (Cable)</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1307,31 +1244,28 @@
           <t>Single Arm Cable Row</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1355,31 +1289,28 @@
           <t>Single Arm Cable Row</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1403,31 +1334,28 @@
           <t>Single Arm Cable Row</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1451,31 +1379,28 @@
           <t>Treadmill</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
         <is>
           <t>0.81</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>90.0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1499,31 +1424,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>50.0</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1547,31 +1469,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>50.0</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1595,31 +1514,28 @@
           <t>Leg Press (Machine)</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>50.0</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1643,31 +1559,28 @@
           <t>Goblet Squat</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1691,31 +1604,28 @@
           <t>Goblet Squat</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1739,31 +1649,28 @@
           <t>Goblet Squat</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1787,27 +1694,24 @@
           <t>Reverse Lunge</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1831,27 +1735,24 @@
           <t>Reverse Lunge</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1875,27 +1776,24 @@
           <t>Reverse Lunge</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1919,31 +1817,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>25.0</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1967,31 +1862,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2015,31 +1907,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2063,27 +1952,24 @@
           <t>Single Leg Standing Calf Raise (Barbell)</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2107,27 +1993,24 @@
           <t>Single Leg Standing Calf Raise (Barbell)</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2151,27 +2034,24 @@
           <t>Single Leg Standing Calf Raise (Barbell)</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2195,31 +2075,28 @@
           <t>Treadmill</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr">
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
         <is>
           <t>0.5</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>600.0</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2243,27 +2120,24 @@
           <t>Bench Press (Barbell)</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2287,27 +2161,24 @@
           <t>Bench Press (Barbell)</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2331,27 +2202,24 @@
           <t>Bench Press (Barbell)</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2375,31 +2243,28 @@
           <t>Shoulder Press (Machine Plates)</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>30.0</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2423,31 +2288,28 @@
           <t>Shoulder Press (Machine Plates)</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>30.0</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2471,31 +2333,28 @@
           <t>Shoulder Press (Machine Plates)</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2519,31 +2378,28 @@
           <t>Butterfly (Pec Deck)</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2567,31 +2423,28 @@
           <t>Butterfly (Pec Deck)</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>50.0</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2615,31 +2468,28 @@
           <t>Butterfly (Pec Deck)</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>40.0</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2663,31 +2513,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2711,31 +2558,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2759,31 +2603,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2807,31 +2648,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>25.0</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2855,31 +2693,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2903,31 +2738,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+          <t>11.0</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2951,27 +2783,24 @@
           <t>Squat (Barbell)</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2995,31 +2824,28 @@
           <t>Squat (Barbell)</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3043,27 +2869,24 @@
           <t>Squat (Barbell)</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr">
         <is>
-          <t>normal</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3087,31 +2910,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3135,31 +2955,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3183,31 +3000,28 @@
           <t>Lying Leg Curl (Machine)</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3231,31 +3045,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>80.0</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3279,31 +3090,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3327,31 +3135,28 @@
           <t>Calf Extension (Machine)</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Program is just about ready for graphing. Technically stuff is being graphed right now but it needs to be prettier.
</commit_message>
<xml_diff>
--- a/workouts.xlsx
+++ b/workouts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,11 +433,14 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D1" t="n">
         <v>8</v>
       </c>
+      <c r="E1" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -451,11 +454,14 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
       </c>
+      <c r="E2" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -469,11 +475,14 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
       </c>
+      <c r="E3" t="n">
+        <v>315</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -487,10 +496,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="5">
@@ -505,10 +517,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
         <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -523,11 +538,14 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
       </c>
+      <c r="E6" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -541,11 +559,14 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>10</v>
       </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -559,11 +580,14 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
         <v>5</v>
       </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -577,11 +601,14 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
       </c>
+      <c r="E9" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -595,10 +622,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D10" t="n">
         <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>360</v>
       </c>
     </row>
     <row r="11">
@@ -613,11 +643,14 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D11" t="n">
         <v>7</v>
       </c>
+      <c r="E11" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -631,10 +664,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D12" t="n">
         <v>6</v>
+      </c>
+      <c r="E12" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="13">
@@ -649,11 +685,14 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
       </c>
+      <c r="E13" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -667,11 +706,14 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
         <v>7</v>
       </c>
+      <c r="E14" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -685,10 +727,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D15" t="n">
         <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="16">
@@ -703,11 +748,14 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D16" t="n">
         <v>10</v>
       </c>
+      <c r="E16" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -721,11 +769,14 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D17" t="n">
         <v>10</v>
       </c>
+      <c r="E17" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -739,10 +790,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D18" t="n">
         <v>6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>420</v>
       </c>
     </row>
     <row r="19">
@@ -757,11 +811,14 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D19" t="n">
         <v>10</v>
       </c>
+      <c r="E19" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -775,11 +832,14 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D20" t="n">
         <v>10</v>
       </c>
+      <c r="E20" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -793,11 +853,14 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D21" t="n">
         <v>8</v>
       </c>
+      <c r="E21" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -811,11 +874,14 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
       </c>
+      <c r="E22" t="n">
+        <v>280</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -829,10 +895,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D23" t="n">
         <v>6</v>
+      </c>
+      <c r="E23" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="24">
@@ -847,11 +916,14 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D24" t="n">
         <v>8</v>
       </c>
+      <c r="E24" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -865,10 +937,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D25" t="n">
         <v>6</v>
+      </c>
+      <c r="E25" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="26">
@@ -883,10 +958,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D26" t="n">
         <v>6</v>
+      </c>
+      <c r="E26" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="27">
@@ -901,10 +979,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D27" t="n">
         <v>6</v>
+      </c>
+      <c r="E27" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="28">
@@ -919,10 +1000,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D28" t="n">
         <v>6</v>
+      </c>
+      <c r="E28" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="29">
@@ -937,10 +1021,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
         <v>6</v>
+      </c>
+      <c r="E29" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -955,10 +1042,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D30" t="n">
         <v>6</v>
+      </c>
+      <c r="E30" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -973,10 +1063,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
         <v>6</v>
+      </c>
+      <c r="E31" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="32">
@@ -991,10 +1084,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="D32" t="n">
         <v>6</v>
+      </c>
+      <c r="E32" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="33">
@@ -1009,10 +1105,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="D33" t="n">
         <v>6</v>
+      </c>
+      <c r="E33" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="34">
@@ -1027,11 +1126,14 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>12.5</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
       </c>
+      <c r="E34" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1045,11 +1147,14 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D35" t="n">
         <v>8</v>
       </c>
+      <c r="E35" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1063,11 +1168,14 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D36" t="n">
         <v>8</v>
       </c>
+      <c r="E36" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1081,11 +1189,14 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D37" t="n">
         <v>8</v>
       </c>
+      <c r="E37" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1099,11 +1210,14 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D38" t="n">
         <v>7</v>
       </c>
+      <c r="E38" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1117,11 +1231,14 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
       </c>
+      <c r="E39" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1135,11 +1252,14 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D40" t="n">
         <v>7</v>
       </c>
+      <c r="E40" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1153,10 +1273,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
         <v>6</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1171,10 +1294,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
         <v>6</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1189,10 +1315,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1207,11 +1336,14 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D44" t="n">
         <v>10</v>
       </c>
+      <c r="E44" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1225,11 +1357,14 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D45" t="n">
         <v>10</v>
       </c>
+      <c r="E45" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1243,11 +1378,14 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D46" t="n">
         <v>10</v>
       </c>
+      <c r="E46" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1261,11 +1399,14 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>8</v>
       </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1279,11 +1420,14 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
         <v>8</v>
       </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1293,12 +1437,18 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Treadmill</t>
+          <t>Single Leg Standing Calf Raise (Barbell)</t>
         </is>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
+      <c r="D49" t="n">
+        <v>10</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1312,10 +1462,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D50" t="n">
         <v>6</v>
+      </c>
+      <c r="E50" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="51">
@@ -1330,10 +1483,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
+      </c>
+      <c r="E51" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="52">
@@ -1348,11 +1504,14 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D52" t="n">
         <v>7</v>
       </c>
+      <c r="E52" t="n">
+        <v>245</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1366,10 +1525,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D53" t="n">
         <v>6</v>
+      </c>
+      <c r="E53" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="54">
@@ -1384,10 +1546,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D54" t="n">
         <v>6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="55">
@@ -1402,10 +1567,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
+      </c>
+      <c r="E55" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="56">
@@ -1420,11 +1588,14 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D56" t="n">
         <v>5</v>
       </c>
+      <c r="E56" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1438,11 +1609,14 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D57" t="n">
         <v>5</v>
       </c>
+      <c r="E57" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1456,10 +1630,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D58" t="n">
         <v>6</v>
+      </c>
+      <c r="E58" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="59">
@@ -1474,11 +1651,14 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D59" t="n">
         <v>10</v>
       </c>
+      <c r="E59" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1492,11 +1672,14 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D60" t="n">
         <v>10</v>
       </c>
+      <c r="E60" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1510,11 +1693,14 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D61" t="n">
         <v>8</v>
       </c>
+      <c r="E61" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1528,11 +1714,14 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D62" t="n">
         <v>10</v>
       </c>
+      <c r="E62" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1546,11 +1735,14 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D63" t="n">
         <v>10</v>
       </c>
+      <c r="E63" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1564,11 +1756,14 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D64" t="n">
         <v>11</v>
       </c>
+      <c r="E64" t="n">
+        <v>385</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1582,11 +1777,14 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>10</v>
       </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1600,11 +1798,14 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D66" t="n">
         <v>10</v>
       </c>
+      <c r="E66" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1618,10 +1819,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
         <v>6</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1636,11 +1840,14 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D68" t="n">
         <v>8</v>
       </c>
+      <c r="E68" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1654,11 +1861,14 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D69" t="n">
         <v>8</v>
       </c>
+      <c r="E69" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1672,11 +1882,14 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D70" t="n">
         <v>8</v>
       </c>
+      <c r="E70" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1690,10 +1903,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D71" t="n">
         <v>6</v>
+      </c>
+      <c r="E71" t="n">
+        <v>480</v>
       </c>
     </row>
     <row r="72">
@@ -1708,11 +1924,14 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D72" t="n">
         <v>8</v>
       </c>
+      <c r="E72" t="n">
+        <v>480</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1726,10 +1945,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D73" t="n">
         <v>6</v>
+      </c>
+      <c r="E73" t="n">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>